<commit_message>
Added weighting feature to FBGNeedle file and ran optimization
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_3CH_4AA/Jig_Calibration_08-05-20/Data Matrices_new_proc.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_3CH_4AA/Jig_Calibration_08-05-20/Data Matrices_new_proc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="24">
   <si>
     <t>Row</t>
   </si>
@@ -109,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -125,11 +125,51 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -139,6 +179,46 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,39 +244,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="41" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -228,7 +308,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -260,7 +340,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -292,7 +372,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -324,7 +404,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -356,7 +436,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -388,7 +468,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="41" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -420,7 +500,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -452,7 +532,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -484,7 +564,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -516,7 +596,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="41" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -548,7 +628,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -580,7 +660,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -612,7 +692,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -665,39 +745,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="43" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -729,7 +809,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -761,7 +841,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -793,7 +873,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -825,7 +905,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -857,7 +937,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -889,7 +969,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="43" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -921,7 +1001,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -953,7 +1033,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -985,7 +1065,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="43" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1017,7 +1097,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -1049,7 +1129,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="43" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -1081,7 +1161,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -1113,7 +1193,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -1166,39 +1246,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="45" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1230,7 +1310,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1262,7 +1342,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1294,7 +1374,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1326,7 +1406,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1358,7 +1438,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1390,7 +1470,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="45" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1422,7 +1502,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1454,7 +1534,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1486,7 +1566,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1518,7 +1598,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -1550,7 +1630,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -1582,7 +1662,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -1614,7 +1694,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -1667,39 +1747,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="47" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1731,7 +1811,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1763,7 +1843,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1795,7 +1875,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1827,7 +1907,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1859,7 +1939,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="47" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1891,7 +1971,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="47" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1923,7 +2003,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1955,7 +2035,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="47" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1987,7 +2067,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -2019,7 +2099,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="47" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -2051,7 +2131,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="47" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -2083,7 +2163,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="47" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -2115,7 +2195,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B15">

</xml_diff>